<commit_message>
Add InvoiceType to documentation
</commit_message>
<xml_diff>
--- a/Guia_Api_Facturas_Generix_ADT.xlsx
+++ b/Guia_Api_Facturas_Generix_ADT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://generixgrouponline-my.sharepoint.com/personal/layuso_generixgroup_com/Documents/Documentos/factura/ADT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{DED31407-6595-4F0D-AFCF-B2C379325484}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{704DE48E-9FD0-4DC1-B2FE-10A5D38E08A8}"/>
+  <xr:revisionPtr revIDLastSave="54" documentId="13_ncr:1_{DED31407-6595-4F0D-AFCF-B2C379325484}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EBF730B1-DC94-4431-8E27-D927B8FF7837}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Esquema General" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1630" uniqueCount="617">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1642" uniqueCount="622">
   <si>
     <t>JSON</t>
   </si>
@@ -1759,9 +1759,6 @@
     <t>2.2.5.1.16.3.</t>
   </si>
   <si>
-    <t>2.2.5.1.16.3.1.</t>
-  </si>
-  <si>
     <t>2.2.5.1.16.3.2.</t>
   </si>
   <si>
@@ -1913,13 +1910,31 @@
     <t>BICType string positions: 11</t>
   </si>
   <si>
-    <t>PaymentReconciliationReferenc e</t>
-  </si>
-  <si>
     <t>2.2.6.1.4.2.</t>
   </si>
   <si>
     <t>Referencia expresa del pago. Dato que precisa el Emisor para conciliar los pagos con cada factura.</t>
+  </si>
+  <si>
+    <t>PaymentReconciliationReference</t>
+  </si>
+  <si>
+    <t>2.2.5.1.16.3.7.</t>
+  </si>
+  <si>
+    <t>2.2.6.1.6.</t>
+  </si>
+  <si>
+    <t>CollectionAdditionalInformation</t>
+  </si>
+  <si>
+    <t>Observaciones de cobro. Libre para uso del Emisor.</t>
+  </si>
+  <si>
+    <t>2.2.8.2.3.</t>
+  </si>
+  <si>
+    <t>Tipo de Factura</t>
   </si>
 </sst>
 </file>
@@ -2466,7 +2481,7 @@
       <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="86264" y="94890"/>
-          <a:ext cx="1309458" cy="289955"/>
+          <a:ext cx="1267943" cy="289955"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2801,7 +2816,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:G2"/>
     </sheetView>
   </sheetViews>
@@ -2913,7 +2928,7 @@
       </c>
       <c r="H6" s="29"/>
     </row>
-    <row r="7" spans="1:9" ht="36" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="26"/>
       <c r="B7" s="15" t="s">
         <v>345</v>
@@ -5135,10 +5150,10 @@
         <v>412</v>
       </c>
       <c r="C29" s="20" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="D29" s="43" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="E29" s="17"/>
       <c r="F29" s="26" t="s">
@@ -5176,7 +5191,7 @@
     <row r="31" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A31" s="16"/>
       <c r="B31" s="20" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="C31" s="20" t="s">
         <v>14</v>
@@ -5198,7 +5213,7 @@
     <row r="32" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A32" s="16"/>
       <c r="B32" s="20" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="C32" s="20" t="s">
         <v>15</v>
@@ -5220,7 +5235,7 @@
     <row r="33" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A33" s="16"/>
       <c r="B33" s="20" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="C33" s="20" t="s">
         <v>16</v>
@@ -5242,7 +5257,7 @@
     <row r="34" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A34" s="16"/>
       <c r="B34" s="20" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="C34" s="20" t="s">
         <v>17</v>
@@ -5264,7 +5279,7 @@
     <row r="35" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A35" s="16"/>
       <c r="B35" s="20" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="C35" s="20" t="s">
         <v>18</v>
@@ -5286,7 +5301,7 @@
     <row r="36" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A36" s="16"/>
       <c r="B36" s="20" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="C36" s="20" t="s">
         <v>19</v>
@@ -5308,7 +5323,7 @@
     <row r="37" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A37" s="16"/>
       <c r="B37" s="20" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="C37" s="20" t="s">
         <v>20</v>
@@ -5462,7 +5477,7 @@
     <row r="44" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A44" s="16"/>
       <c r="B44" s="20" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C44" s="20" t="s">
         <v>27</v>
@@ -5484,7 +5499,7 @@
     <row r="45" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A45" s="16"/>
       <c r="B45" s="20" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C45" s="20" t="s">
         <v>28</v>
@@ -5506,7 +5521,7 @@
     <row r="46" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A46" s="16"/>
       <c r="B46" s="20" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="C46" s="20" t="s">
         <v>29</v>
@@ -5528,7 +5543,7 @@
     <row r="47" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A47" s="16"/>
       <c r="B47" s="20" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="C47" s="20" t="s">
         <v>30</v>
@@ -5550,7 +5565,7 @@
     <row r="48" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A48" s="16"/>
       <c r="B48" s="20" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="C48" s="20" t="s">
         <v>31</v>
@@ -5572,7 +5587,7 @@
     <row r="49" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A49" s="16"/>
       <c r="B49" s="20" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="C49" s="20" t="s">
         <v>32</v>
@@ -6301,9 +6316,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25333C4E-FCEB-4BCB-A95F-5DF88E54B42A}">
-  <dimension ref="A1:I125"/>
+  <dimension ref="A1:I127"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:H2"/>
     </sheetView>
   </sheetViews>
@@ -8429,14 +8444,14 @@
         <v>562</v>
       </c>
       <c r="C97" s="20" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="D97" s="43" t="s">
         <v>236</v>
       </c>
       <c r="E97" s="17"/>
       <c r="F97" s="44" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="G97" s="44" t="s">
         <v>141</v>
@@ -8451,7 +8466,7 @@
         <v>563</v>
       </c>
       <c r="C98" s="20" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D98" s="43" t="s">
         <v>192</v>
@@ -8464,7 +8479,7 @@
         <v>129</v>
       </c>
       <c r="H98" s="43" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="99" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -8473,7 +8488,7 @@
         <v>564</v>
       </c>
       <c r="C99" s="20" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D99" s="43" t="s">
         <v>192</v>
@@ -8536,7 +8551,7 @@
     <row r="102" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A102" s="15"/>
       <c r="B102" s="15" t="s">
-        <v>567</v>
+        <v>590</v>
       </c>
       <c r="C102" s="20" t="s">
         <v>25</v>
@@ -8558,7 +8573,7 @@
     <row r="103" spans="1:8" ht="24" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A103" s="15"/>
       <c r="B103" s="15" t="s">
-        <v>591</v>
+        <v>616</v>
       </c>
       <c r="C103" s="20" t="s">
         <v>26</v>
@@ -8734,13 +8749,13 @@
     <row r="111" spans="1:8" ht="24" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A111" s="15"/>
       <c r="B111" s="15" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="C111" s="15" t="s">
+        <v>610</v>
+      </c>
+      <c r="D111" s="2" t="s">
         <v>611</v>
-      </c>
-      <c r="D111" s="2" t="s">
-        <v>612</v>
       </c>
       <c r="E111" s="26"/>
       <c r="F111" s="26" t="s">
@@ -8750,7 +8765,7 @@
         <v>141</v>
       </c>
       <c r="H111" s="16" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="112" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -8759,10 +8774,10 @@
         <v>511</v>
       </c>
       <c r="C112" s="15" t="s">
-        <v>614</v>
+        <v>618</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>616</v>
+        <v>619</v>
       </c>
       <c r="E112" s="26"/>
       <c r="F112" s="26" t="s">
@@ -8771,196 +8786,196 @@
       <c r="G112" s="26" t="s">
         <v>141</v>
       </c>
-      <c r="H112" s="16" t="s">
+      <c r="H112" s="26" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="15"/>
+      <c r="B113" s="15" t="s">
+        <v>617</v>
+      </c>
+      <c r="C113" s="15" t="s">
+        <v>615</v>
+      </c>
+      <c r="D113" s="2" t="s">
+        <v>614</v>
+      </c>
+      <c r="E113" s="26"/>
+      <c r="F113" s="26" t="s">
+        <v>140</v>
+      </c>
+      <c r="G113" s="26" t="s">
+        <v>141</v>
+      </c>
+      <c r="H113" s="16" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="113" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="37"/>
-      <c r="B113" s="37" t="s">
+    <row r="114" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="37"/>
+      <c r="B114" s="37" t="s">
         <v>360</v>
       </c>
-      <c r="C113" s="37" t="s">
+      <c r="C114" s="37" t="s">
+        <v>593</v>
+      </c>
+      <c r="D114" s="40" t="s">
         <v>594</v>
       </c>
-      <c r="D113" s="40" t="s">
+      <c r="E114" s="39"/>
+      <c r="F114" s="39" t="s">
+        <v>140</v>
+      </c>
+      <c r="G114" s="39" t="s">
+        <v>141</v>
+      </c>
+      <c r="H114" s="38" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" ht="24" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A115" s="15"/>
+      <c r="B115" s="15" t="s">
+        <v>512</v>
+      </c>
+      <c r="C115" s="15" t="s">
         <v>595</v>
       </c>
-      <c r="E113" s="39"/>
-      <c r="F113" s="39" t="s">
+      <c r="D115" s="2" t="s">
+        <v>596</v>
+      </c>
+      <c r="E115" s="26"/>
+      <c r="F115" s="26" t="s">
+        <v>586</v>
+      </c>
+      <c r="G115" s="26" t="s">
+        <v>141</v>
+      </c>
+      <c r="H115" s="17" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="37"/>
+      <c r="B116" s="37" t="s">
+        <v>599</v>
+      </c>
+      <c r="C116" s="37" t="s">
+        <v>113</v>
+      </c>
+      <c r="D116" s="40" t="s">
+        <v>164</v>
+      </c>
+      <c r="E116" s="39"/>
+      <c r="F116" s="39" t="s">
         <v>140</v>
       </c>
-      <c r="G113" s="39" t="s">
+      <c r="G116" s="39" t="s">
         <v>141</v>
       </c>
-      <c r="H113" s="38" t="s">
-        <v>599</v>
-      </c>
-    </row>
-    <row r="114" spans="1:8" ht="24" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="15"/>
-      <c r="B114" s="15" t="s">
-        <v>512</v>
-      </c>
-      <c r="C114" s="15" t="s">
-        <v>596</v>
-      </c>
-      <c r="D114" s="2" t="s">
-        <v>597</v>
-      </c>
-      <c r="E114" s="26"/>
-      <c r="F114" s="26" t="s">
-        <v>587</v>
-      </c>
-      <c r="G114" s="26" t="s">
-        <v>141</v>
-      </c>
-      <c r="H114" s="17" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="115" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="37"/>
-      <c r="B115" s="37" t="s">
-        <v>600</v>
-      </c>
-      <c r="C115" s="37" t="s">
-        <v>113</v>
-      </c>
-      <c r="D115" s="40" t="s">
-        <v>164</v>
-      </c>
-      <c r="E115" s="39"/>
-      <c r="F115" s="39" t="s">
-        <v>140</v>
-      </c>
-      <c r="G115" s="39" t="s">
-        <v>141</v>
-      </c>
-      <c r="H115" s="38" t="s">
+      <c r="H116" s="38" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="116" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="15"/>
-      <c r="B116" s="15" t="s">
-        <v>601</v>
-      </c>
-      <c r="C116" s="15" t="s">
-        <v>114</v>
-      </c>
-      <c r="D116" s="2" t="s">
-        <v>330</v>
-      </c>
-      <c r="E116" s="26"/>
-      <c r="F116" s="26" t="s">
-        <v>140</v>
-      </c>
-      <c r="G116" s="26" t="s">
-        <v>141</v>
-      </c>
-      <c r="H116" s="16" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="117" spans="1:8" ht="24" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A117" s="15"/>
       <c r="B117" s="15" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="C117" s="15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="E117" s="26"/>
       <c r="F117" s="26" t="s">
-        <v>128</v>
+        <v>140</v>
       </c>
       <c r="G117" s="26" t="s">
-        <v>129</v>
+        <v>141</v>
       </c>
       <c r="H117" s="16" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="118" spans="1:8" ht="24" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A118" s="15"/>
       <c r="B118" s="15" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="C118" s="15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="E118" s="26"/>
       <c r="F118" s="26" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="G118" s="26" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="H118" s="16" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="119" spans="1:8" ht="24" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A119" s="15"/>
       <c r="B119" s="15" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="C119" s="15" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>336</v>
-      </c>
-      <c r="E119" s="24"/>
+        <v>334</v>
+      </c>
+      <c r="E119" s="26"/>
       <c r="F119" s="26" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="G119" s="26" t="s">
-        <v>129</v>
+        <v>141</v>
       </c>
       <c r="H119" s="16" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="120" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" ht="24" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A120" s="15"/>
       <c r="B120" s="15" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="C120" s="15" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>338</v>
-      </c>
-      <c r="E120" s="26"/>
+        <v>336</v>
+      </c>
+      <c r="E120" s="24"/>
       <c r="F120" s="26" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="G120" s="26" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="H120" s="16" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="121" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A121" s="15"/>
       <c r="B121" s="15" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="C121" s="15" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="E121" s="26"/>
       <c r="F121" s="26" t="s">
@@ -8970,95 +8985,139 @@
         <v>141</v>
       </c>
       <c r="H121" s="16" t="s">
-        <v>239</v>
+        <v>339</v>
       </c>
     </row>
     <row r="122" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A122" s="15"/>
       <c r="B122" s="15" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="C122" s="15" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D122" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E122" s="26"/>
       <c r="F122" s="26" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="G122" s="26" t="s">
-        <v>129</v>
+        <v>141</v>
       </c>
       <c r="H122" s="16" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="123" spans="1:8" ht="24" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A123" s="15"/>
       <c r="B123" s="15" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="C123" s="15" t="s">
-        <v>559</v>
+        <v>120</v>
       </c>
       <c r="D123" s="2" t="s">
-        <v>560</v>
+        <v>341</v>
       </c>
       <c r="E123" s="26"/>
       <c r="F123" s="26" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="G123" s="26" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="H123" s="16" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="124" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" ht="24" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A124" s="15"/>
       <c r="B124" s="15" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="C124" s="15" t="s">
-        <v>592</v>
+        <v>559</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>570</v>
+        <v>560</v>
       </c>
       <c r="E124" s="26"/>
-      <c r="F124" s="44" t="s">
-        <v>587</v>
-      </c>
-      <c r="G124" s="44" t="s">
+      <c r="F124" s="26" t="s">
+        <v>140</v>
+      </c>
+      <c r="G124" s="26" t="s">
         <v>141</v>
       </c>
       <c r="H124" s="16" t="s">
-        <v>568</v>
+        <v>561</v>
       </c>
     </row>
     <row r="125" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A125" s="15"/>
       <c r="B125" s="15" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="C125" s="15" t="s">
-        <v>593</v>
+        <v>146</v>
       </c>
       <c r="D125" s="2" t="s">
+        <v>621</v>
+      </c>
+      <c r="E125" s="26"/>
+      <c r="F125" s="26" t="s">
+        <v>140</v>
+      </c>
+      <c r="G125" s="26" t="s">
+        <v>141</v>
+      </c>
+      <c r="H125" s="16" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A126" s="15"/>
+      <c r="B126" s="15" t="s">
+        <v>609</v>
+      </c>
+      <c r="C126" s="15" t="s">
+        <v>591</v>
+      </c>
+      <c r="D126" s="2" t="s">
         <v>569</v>
       </c>
-      <c r="E125" s="26"/>
-      <c r="F125" s="44" t="s">
-        <v>587</v>
-      </c>
-      <c r="G125" s="44" t="s">
+      <c r="E126" s="26"/>
+      <c r="F126" s="44" t="s">
+        <v>586</v>
+      </c>
+      <c r="G126" s="44" t="s">
         <v>141</v>
       </c>
-      <c r="H125" s="16" t="s">
+      <c r="H126" s="16" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A127" s="15"/>
+      <c r="B127" s="15" t="s">
+        <v>620</v>
+      </c>
+      <c r="C127" s="15" t="s">
+        <v>592</v>
+      </c>
+      <c r="D127" s="2" t="s">
         <v>568</v>
+      </c>
+      <c r="E127" s="26"/>
+      <c r="F127" s="44" t="s">
+        <v>586</v>
+      </c>
+      <c r="G127" s="44" t="s">
+        <v>141</v>
+      </c>
+      <c r="H127" s="16" t="s">
+        <v>567</v>
       </c>
     </row>
   </sheetData>
@@ -9067,7 +9126,8 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>